<commit_message>
Created all the pivot tables and charts needed for the dashboard.
</commit_message>
<xml_diff>
--- a/excel_dashboards_challenge.xlsx
+++ b/excel_dashboards_challenge.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jurajkapasny/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanferns/Documents/Data_Science/lighthouse_labs_training/DS_auticon_dataviz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99058CDA-53F7-D443-9234-B2BE0850CC31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B457AA00-4D95-7F4B-8887-6B09C76DDC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="500" windowWidth="14700" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data_values" sheetId="2" r:id="rId2"/>
+    <sheet name="year_and_region_pivot" sheetId="3" r:id="rId3"/>
+    <sheet name="product_pivot" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="chtProductBreakup">IF(valProductPicked="",#REF!,#REF!)</definedName>
-    <definedName name="lstProducts">data!$H$2:$H$7</definedName>
-    <definedName name="lstRegions">data!$I$2:$I$3</definedName>
-    <definedName name="lstYears">data!$G$2:$G$12</definedName>
+    <definedName name="lstProducts">data_values!$B$2:$B$7</definedName>
+    <definedName name="lstRegions">data_values!$C$2:$C$3</definedName>
+    <definedName name="lstYears">data_values!$A$2:$A$12</definedName>
     <definedName name="plstProducts">#REF!</definedName>
     <definedName name="plstRegions">#REF!</definedName>
     <definedName name="plstYears">#REF!</definedName>
@@ -31,6 +34,9 @@
     <definedName name="valYearPicked">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="19">
   <si>
     <t>Year</t>
   </si>
@@ -91,6 +97,18 @@
   </si>
   <si>
     <t>South</t>
+  </si>
+  <si>
+    <t>Sum of Sales ($)</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
   </si>
 </sst>
 </file>
@@ -155,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +183,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -187,6 +209,3504 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[excel_dashboards_challenge.xlsx]year_and_region_pivot!Year&amp;RegionPivot</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Sales by Year</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> and Region</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>year_and_region_pivot!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>South</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>year_and_region_pivot!$A$5:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>year_and_region_pivot!$B$5:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8660</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8610</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8790</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7900</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8540</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7870</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9940</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8590</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8760</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E921-3048-83E8-50744B4BABE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>year_and_region_pivot!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>North</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>year_and_region_pivot!$A$5:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2001</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>year_and_region_pivot!$C$5:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6430</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6350</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5610</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5860</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6090</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6560</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E921-3048-83E8-50744B4BABE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="113"/>
+        <c:axId val="1394543376"/>
+        <c:axId val="1394512720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1394543376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394512720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1394512720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sales</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394543376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[excel_dashboards_challenge.xlsx]product_pivot!ProductPivot</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Sales by Product</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>product_pivot!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>product_pivot!$A$4:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Biscuits</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chocochips</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chocolates</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cookies</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jelly Beans</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Nutri Bars</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>product_pivot!$B$4:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>27260</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26770</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28050</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1CF0-1D4A-90C5-89D2620414AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1501946272"/>
+        <c:axId val="1501760848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1501946272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Product Types</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501760848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1501760848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sales ($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501946272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1000"/>
+        <c:minorUnit val="100"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88032</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100444</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>425738</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>108238</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A6231F-FC4A-CE80-E608-936475E503B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>759112</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>497897</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6607EDD-DAD2-AAA6-7734-F588D1FA629A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45413.670317476855" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="132" xr:uid="{447281EB-B7DA-F24D-A566-E201B9F9B69C}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="tblSales"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2001" maxValue="2011" count="11">
+        <n v="2001"/>
+        <n v="2002"/>
+        <n v="2003"/>
+        <n v="2004"/>
+        <n v="2005"/>
+        <n v="2006"/>
+        <n v="2007"/>
+        <n v="2008"/>
+        <n v="2009"/>
+        <n v="2010"/>
+        <n v="2011"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Product" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Biscuits"/>
+        <s v="Chocolates"/>
+        <s v="Chocochips"/>
+        <s v="Cookies"/>
+        <s v="Nutri Bars"/>
+        <s v="Jelly Beans"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="2">
+        <s v="North"/>
+        <s v="South"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sales ($)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="780" maxValue="2100"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="132">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1140"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1800"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="950"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1570"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1120"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1510"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1040"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1350"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="930"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1210"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="920"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1320"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1210"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1370"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1110"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1370"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="990"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1480"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1160"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1350"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="980"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1280"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1110"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1740"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="880"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1350"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="990"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1110"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1140"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="820"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="970"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1600"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="920"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1870"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1080"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1430"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="860"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1470"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1080"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1950"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1050"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1940"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="890"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1840"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1230"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1550"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1190"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="950"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1420"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1140"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1090"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="980"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1600"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1010"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1290"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1060"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1490"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="950"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="980"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1050"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1490"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1030"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1460"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="860"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1050"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="910"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1430"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="950"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1320"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1060"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1790"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1020"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1480"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="980"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1400"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="890"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1760"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="970"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1190"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="870"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1010"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="880"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1260"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1070"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1590"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="890"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1430"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1050"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="780"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1120"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1220"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="950"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1260"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1120"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1620"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="850"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1390"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1150"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1470"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1080"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1260"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1110"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1810"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="950"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1460"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1180"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1400"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1010"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1420"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="970"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1370"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1100"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1360"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1120"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1380"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1020"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="980"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1130"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="2100"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1080"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1360"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="920"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1020"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1200"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1750"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1060"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1070"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1080"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1760"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1090"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1700"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="12">
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales ($)" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="7">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales ($)" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblSales" displayName="tblSales" ref="A1:D133" totalsRowShown="0">
   <autoFilter ref="A1:D133" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -201,9 +3721,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,9 +3761,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,26 +3796,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -328,26 +3831,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,9 +4010,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="152" zoomScaleNormal="152" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -548,15 +4032,6 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -571,15 +4046,6 @@
       <c r="D2">
         <v>1140</v>
       </c>
-      <c r="G2" s="2">
-        <v>2001</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -596,15 +4062,6 @@
       <c r="D3">
         <v>1800</v>
       </c>
-      <c r="G3" s="2">
-        <v>2002</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -619,13 +4076,6 @@
       <c r="D4">
         <v>950</v>
       </c>
-      <c r="G4" s="2">
-        <v>2003</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -640,13 +4090,6 @@
       <c r="D5">
         <v>1570</v>
       </c>
-      <c r="G5" s="2">
-        <v>2004</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -661,13 +4104,6 @@
       <c r="D6">
         <v>1120</v>
       </c>
-      <c r="G6" s="2">
-        <v>2005</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -682,12 +4118,6 @@
       <c r="D7">
         <v>1510</v>
       </c>
-      <c r="G7" s="2">
-        <v>2006</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -702,10 +4132,6 @@
       <c r="D8">
         <v>1040</v>
       </c>
-      <c r="G8" s="2">
-        <v>2007</v>
-      </c>
-      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -720,11 +4146,6 @@
       <c r="D9">
         <v>1350</v>
       </c>
-      <c r="G9" s="2">
-        <v>2008</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -739,11 +4160,6 @@
       <c r="D10">
         <v>930</v>
       </c>
-      <c r="G10" s="2">
-        <v>2009</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -758,11 +4174,6 @@
       <c r="D11">
         <v>1210</v>
       </c>
-      <c r="G11" s="2">
-        <v>2010</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -777,11 +4188,6 @@
       <c r="D12">
         <v>920</v>
       </c>
-      <c r="G12" s="2">
-        <v>2011</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -2484,4 +5890,417 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA82B3EB-B65A-FE46-A46A-3294A6CF99B2}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08339962-434C-CD47-9FEE-C49A2125B0E3}">
+  <dimension ref="A3:D16"/>
+  <sheetViews>
+    <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2011</v>
+      </c>
+      <c r="B5">
+        <v>8660</v>
+      </c>
+      <c r="C5">
+        <v>6430</v>
+      </c>
+      <c r="D5">
+        <v>15090</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>2010</v>
+      </c>
+      <c r="B6">
+        <v>8610</v>
+      </c>
+      <c r="C6">
+        <v>6350</v>
+      </c>
+      <c r="D6">
+        <v>14960</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>2009</v>
+      </c>
+      <c r="B7">
+        <v>8790</v>
+      </c>
+      <c r="C7">
+        <v>6320</v>
+      </c>
+      <c r="D7">
+        <v>15110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>2008</v>
+      </c>
+      <c r="B8">
+        <v>7900</v>
+      </c>
+      <c r="C8">
+        <v>6200</v>
+      </c>
+      <c r="D8">
+        <v>14100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>2007</v>
+      </c>
+      <c r="B9">
+        <v>8100</v>
+      </c>
+      <c r="C9">
+        <v>5610</v>
+      </c>
+      <c r="D9">
+        <v>13710</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>2006</v>
+      </c>
+      <c r="B10">
+        <v>8540</v>
+      </c>
+      <c r="C10">
+        <v>5860</v>
+      </c>
+      <c r="D10">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>2005</v>
+      </c>
+      <c r="B11">
+        <v>7870</v>
+      </c>
+      <c r="C11">
+        <v>6090</v>
+      </c>
+      <c r="D11">
+        <v>13960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>2004</v>
+      </c>
+      <c r="B12">
+        <v>9940</v>
+      </c>
+      <c r="C12">
+        <v>6110</v>
+      </c>
+      <c r="D12">
+        <v>16050</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>2003</v>
+      </c>
+      <c r="B13">
+        <v>8180</v>
+      </c>
+      <c r="C13">
+        <v>5980</v>
+      </c>
+      <c r="D13">
+        <v>14160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>2002</v>
+      </c>
+      <c r="B14">
+        <v>8590</v>
+      </c>
+      <c r="C14">
+        <v>6560</v>
+      </c>
+      <c r="D14">
+        <v>15150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>2001</v>
+      </c>
+      <c r="B15">
+        <v>8760</v>
+      </c>
+      <c r="C15">
+        <v>6100</v>
+      </c>
+      <c r="D15">
+        <v>14860</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>93940</v>
+      </c>
+      <c r="C16">
+        <v>67610</v>
+      </c>
+      <c r="D16">
+        <v>161550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F519B4B-0B7B-7E4B-9E0E-012A2C2C772E}">
+  <dimension ref="A3:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>27260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>26770</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>26450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>26890</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>28050</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>26130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>161550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created a new dashboard with slicers from new pivot tables and charts.
</commit_message>
<xml_diff>
--- a/excel_dashboards_challenge.xlsx
+++ b/excel_dashboards_challenge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanferns/Documents/Data_Science/lighthouse_labs_training/DS_auticon_dataviz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47452C29-235A-B944-958B-2FC525597D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E173C-B7B5-894D-81C7-1BF6BCFA60FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,9 @@
     <definedName name="plstRegions">#REF!</definedName>
     <definedName name="plstYears">#REF!</definedName>
     <definedName name="Slicer_Region">#N/A</definedName>
+    <definedName name="Slicer_Region1">#N/A</definedName>
     <definedName name="Slicer_Year">#N/A</definedName>
+    <definedName name="Slicer_Year1">#N/A</definedName>
     <definedName name="valHelpMessage">#REF!</definedName>
     <definedName name="valHelpStatus">#REF!</definedName>
     <definedName name="valProductPicked">#REF!</definedName>
@@ -46,14 +48,16 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
-    <pivotCache cacheId="11" r:id="rId12"/>
+    <pivotCache cacheId="4" r:id="rId11"/>
+    <pivotCache cacheId="5" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
         <x14:slicerCache r:id="rId13"/>
         <x14:slicerCache r:id="rId14"/>
+        <x14:slicerCache r:id="rId15"/>
+        <x14:slicerCache r:id="rId16"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -73,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="23">
   <si>
     <t>Year</t>
   </si>
@@ -223,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,9 +248,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3493,119 +3494,6 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>All Regions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>all_reg_year_and_region_pivot!$A$5:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2001</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>all_reg_year_and_region_pivot!$B$5:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>15090</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14960</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15110</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13710</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14400</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13960</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16050</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14160</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15150</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14860</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7009-C04A-BB58-DF8E57EF8B05}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>all_reg_year_and_region_pivot!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
                   <c:v>South</c:v>
                 </c:pt>
               </c:strCache>
@@ -3623,203 +3511,30 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>all_reg_year_and_region_pivot!$A$5:$A$16</c:f>
+              <c:f>all_reg_year_and_region_pivot!$A$5:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2001</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all_reg_year_and_region_pivot!$C$5:$C$16</c:f>
+              <c:f>all_reg_year_and_region_pivot!$B$5:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>8660</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8610</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8790</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7900</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8540</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7870</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9940</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8590</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7009-C04A-BB58-DF8E57EF8B05}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>all_reg_year_and_region_pivot!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>North</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>all_reg_year_and_region_pivot!$A$5:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2001</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>all_reg_year_and_region_pivot!$D$5:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6430</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6350</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5610</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5860</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6090</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6110</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5980</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6560</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-7009-C04A-BB58-DF8E57EF8B05}"/>
+              <c16:uniqueId val="{00000000-7009-C04A-BB58-DF8E57EF8B05}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4421,89 +4136,6 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>All Regions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>product_and_region_pivot!$A$5:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Biscuits</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Chocochips</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Chocolates</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Cookies</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Jelly Beans</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Nutri Bars</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>product_and_region_pivot!$B$5:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>27260</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26770</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26450</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26890</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28050</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26130</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-766C-8645-8F0B-6DB2F7C7D89F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>product_and_region_pivot!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
                   <c:v>South</c:v>
                 </c:pt>
               </c:strCache>
@@ -4547,117 +4179,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>product_and_region_pivot!$C$5:$C$11</c:f>
+              <c:f>product_and_region_pivot!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16140</c:v>
+                  <c:v>1360</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15310</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15240</c:v>
+                  <c:v>1020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15530</c:v>
+                  <c:v>1070</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16530</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15190</c:v>
+                  <c:v>1760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-766C-8645-8F0B-6DB2F7C7D89F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>product_and_region_pivot!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>North</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>product_and_region_pivot!$A$5:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Biscuits</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Chocochips</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Chocolates</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Cookies</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Jelly Beans</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Nutri Bars</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>product_and_region_pivot!$D$5:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>11120</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11460</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11360</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11520</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10940</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-766C-8645-8F0B-6DB2F7C7D89F}"/>
+              <c16:uniqueId val="{00000000-766C-8645-8F0B-6DB2F7C7D89F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5007,8 +4556,8 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[excel_dashboards_challenge.xlsx]year_and_region_pivot!Year&amp;RegionPivot</c:name>
-    <c:fmtId val="11"/>
+    <c:name>[excel_dashboards_challenge.xlsx]product_and_region_pivot!Product&amp;RegionPivot</c:name>
+    <c:fmtId val="4"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
@@ -5032,17 +4581,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Sales by Year</a:t>
+              <a:t>Sales</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> and Region</a:t>
+              <a:t> by Product and Region</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5081,7 +4626,7 @@
         <c:idx val="0"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -5137,7 +4682,7 @@
         <c:idx val="1"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:srgbClr val="00B0F0"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -5249,7 +4794,7 @@
         <c:idx val="3"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -5417,7 +4962,7 @@
         <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -5473,7 +5018,7 @@
         <c:idx val="7"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
+            <a:srgbClr val="FF0000"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -5527,62 +5072,6 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="8"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="9"/>
         <c:spPr>
           <a:solidFill>
             <a:srgbClr val="00B0F0"/>
@@ -5641,7 +5130,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -5649,7 +5138,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>year_and_region_pivot!$B$3:$B$4</c:f>
+              <c:f>product_and_region_pivot!$B$3:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5670,203 +5159,60 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>year_and_region_pivot!$A$5:$A$16</c:f>
+              <c:f>product_and_region_pivot!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2011</c:v>
+                  <c:v>Biscuits</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2010</c:v>
+                  <c:v>Chocochips</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2009</c:v>
+                  <c:v>Chocolates</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2008</c:v>
+                  <c:v>Cookies</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2007</c:v>
+                  <c:v>Jelly Beans</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2001</c:v>
+                  <c:v>Nutri Bars</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>year_and_region_pivot!$B$5:$B$16</c:f>
+              <c:f>product_and_region_pivot!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8660</c:v>
+                  <c:v>1360</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8610</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8790</c:v>
+                  <c:v>1020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7900</c:v>
+                  <c:v>1070</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8100</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8540</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7870</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9940</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8590</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8760</c:v>
+                  <c:v>1760</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F6E0-724A-A9CF-659C19CD8BF6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>year_and_region_pivot!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>North</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>year_and_region_pivot!$A$5:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2001</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>year_and_region_pivot!$C$5:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6430</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6350</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5610</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5860</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6090</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6110</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5980</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6560</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F6E0-724A-A9CF-659C19CD8BF6}"/>
+              <c16:uniqueId val="{00000000-096A-E541-A1B8-FC3EDBD2BD2C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5878,21 +5224,21 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="113"/>
-        <c:axId val="1394543376"/>
-        <c:axId val="1394512720"/>
+        <c:gapWidth val="219"/>
+        <c:axId val="803837952"/>
+        <c:axId val="803903744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1394543376"/>
+        <c:axId val="803837952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -5909,8 +5255,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Year</a:t>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Product</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5924,7 +5270,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -5966,7 +5312,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5981,7 +5327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1394512720"/>
+        <c:crossAx val="803903744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5989,13 +5335,14 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1394512720"/>
+        <c:axId val="803903744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10000"/>
+          <c:max val="4000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -6013,7 +5360,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -6030,14 +5377,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Sales</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> ($)</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t> </a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6050,7 +5396,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -6070,14 +5416,16 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -6101,9 +5449,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1394543376"/>
+        <c:crossAx val="803837952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="200"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -10507,22 +9856,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>815398</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>337706</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>7794</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BAD2166-A67E-5344-85B5-041FDA92F7D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE023B15-95A6-DA42-AA24-00F7FA1F88C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10540,6 +9889,162 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>168852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533977</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>14431</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Year 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25CFB157-DCD3-C724-91BE-41D44EFC5FC2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Year 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="637886"/>
+              <a:ext cx="1356591" cy="3222625"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>16455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>505113</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28865</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Region 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB35979A-D39F-BF2D-D72F-103CE95E4DE9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="4050148"/>
+              <a:ext cx="1327727" cy="1138092"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10638,7 +10143,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1185299425"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -13031,7 +12536,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -13118,7 +12623,7 @@
   <dataFields count="1">
     <dataField name="Sum of Sales ($)" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="8">
+  <chartFormats count="6">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -13191,30 +12696,6 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="11" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -13229,7 +12710,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0">
@@ -13342,22 +12823,22 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27187173-58F9-8548-A30F-6078862BE245}" name="AllRegions&amp;YearPivot" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="A3:E16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27187173-58F9-8548-A30F-6078862BE245}" name="AllRegions&amp;YearPivot" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
       <items count="12">
         <item x="10"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
+        <item h="1" x="9"/>
+        <item h="1" x="8"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -13365,8 +12846,8 @@
     <pivotField axis="axisCol" showAll="0" sortType="descending">
       <items count="4">
         <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -13384,39 +12865,9 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="2">
     <i>
       <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
     </i>
     <i t="grand">
       <x/>
@@ -13425,15 +12876,9 @@
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
+  <colItems count="2">
     <i>
       <x/>
-    </i>
-    <i>
-      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -13502,10 +12947,25 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{587A5213-1027-174C-93A9-DE62478DE20F}" name="Product&amp;RegionPivot" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A3:E11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{587A5213-1027-174C-93A9-DE62478DE20F}" name="Product&amp;RegionPivot" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+  <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="12">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item x="0"/>
@@ -13520,8 +12980,8 @@
     <pivotField axis="axisCol" showAll="0" sortType="descending">
       <items count="4">
         <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -13565,15 +13025,9 @@
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
+  <colItems count="2">
     <i>
       <x/>
-    </i>
-    <i>
-      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -13582,7 +13036,7 @@
   <dataFields count="1">
     <dataField name="Sum of Sales ($)" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="9">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -13615,6 +13069,78 @@
           </reference>
           <reference field="2" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -13675,10 +13201,61 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Year1" xr10:uid="{6BFD85FE-903B-6F4D-8B38-97D3F7EDAACB}" sourceName="Year">
+  <pivotTables>
+    <pivotTable tabId="11" name="Product&amp;RegionPivot"/>
+    <pivotTable tabId="8" name="AllRegions&amp;YearPivot"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1185299425">
+      <items count="11">
+        <i x="0"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="3"/>
+        <i x="4"/>
+        <i x="5"/>
+        <i x="6"/>
+        <i x="7"/>
+        <i x="8"/>
+        <i x="9"/>
+        <i x="10" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Region1" xr10:uid="{F9E17B89-181B-B94A-9085-1EAE8F6DB270}" sourceName="Region">
+  <pivotTables>
+    <pivotTable tabId="11" name="Product&amp;RegionPivot"/>
+    <pivotTable tabId="8" name="AllRegions&amp;YearPivot"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1185299425">
+      <items count="3">
+        <i x="2"/>
+        <i x="0"/>
+        <i x="1" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
   <slicer name="Year" xr10:uid="{382037B9-A901-8146-90A2-900FD4B7BEB9}" cache="Slicer_Year" caption="Pick a year" rowHeight="230716"/>
   <slicer name="Region" xr10:uid="{FFC2A223-CAB5-F54A-8E38-56CB53ED12FE}" cache="Slicer_Region" caption="Region" rowHeight="230716"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Year 1" xr10:uid="{38DD5498-9402-804C-B8E7-A3CA7EC6D120}" cache="Slicer_Year1" caption="Year" rowHeight="230716"/>
+  <slicer name="Region 1" xr10:uid="{436B51DB-1D6A-CD47-97D3-105DACA7702A}" cache="Slicer_Region1" caption="Region" rowHeight="230716"/>
 </slicers>
 </file>
 
@@ -15884,8 +15461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE7D515-685B-0547-83BA-13F164C46B95}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15919,6 +15496,13 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId2"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -16043,8 +15627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08339962-434C-CD47-9FEE-C49A2125B0E3}">
   <dimension ref="A3:H41"/>
   <sheetViews>
-    <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A7" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -16081,13 +15665,13 @@
       <c r="A5" s="5">
         <v>2011</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>8660</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5">
         <v>6430</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5">
         <v>15090</v>
       </c>
     </row>
@@ -16095,13 +15679,13 @@
       <c r="A6" s="5">
         <v>2010</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>8610</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6">
         <v>6350</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6">
         <v>14960</v>
       </c>
     </row>
@@ -16109,13 +15693,13 @@
       <c r="A7" s="5">
         <v>2009</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>8790</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7">
         <v>6320</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7">
         <v>15110</v>
       </c>
     </row>
@@ -16123,13 +15707,13 @@
       <c r="A8" s="5">
         <v>2008</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8">
         <v>7900</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8">
         <v>6200</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8">
         <v>14100</v>
       </c>
     </row>
@@ -16137,13 +15721,13 @@
       <c r="A9" s="5">
         <v>2007</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>8100</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9">
         <v>5610</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9">
         <v>13710</v>
       </c>
     </row>
@@ -16151,13 +15735,13 @@
       <c r="A10" s="5">
         <v>2006</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
         <v>8540</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10">
         <v>5860</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10">
         <v>14400</v>
       </c>
     </row>
@@ -16165,13 +15749,13 @@
       <c r="A11" s="5">
         <v>2005</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11">
         <v>7870</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11">
         <v>6090</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11">
         <v>13960</v>
       </c>
     </row>
@@ -16179,13 +15763,13 @@
       <c r="A12" s="5">
         <v>2004</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>9940</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12">
         <v>6110</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12">
         <v>16050</v>
       </c>
     </row>
@@ -16193,13 +15777,13 @@
       <c r="A13" s="5">
         <v>2003</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>8180</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13">
         <v>5980</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13">
         <v>14160</v>
       </c>
     </row>
@@ -16207,13 +15791,13 @@
       <c r="A14" s="5">
         <v>2002</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
         <v>8590</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14">
         <v>6560</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14">
         <v>15150</v>
       </c>
     </row>
@@ -16221,13 +15805,13 @@
       <c r="A15" s="5">
         <v>2001</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
         <v>8760</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15">
         <v>6100</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15">
         <v>14860</v>
       </c>
     </row>
@@ -16235,13 +15819,13 @@
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16">
         <v>93940</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16">
         <v>67610</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16">
         <v>161550</v>
       </c>
     </row>
@@ -16304,7 +15888,7 @@
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>27260</v>
       </c>
     </row>
@@ -16312,7 +15896,7 @@
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>26770</v>
       </c>
     </row>
@@ -16320,7 +15904,7 @@
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>26450</v>
       </c>
     </row>
@@ -16328,7 +15912,7 @@
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>26890</v>
       </c>
     </row>
@@ -16336,7 +15920,7 @@
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8">
         <v>28050</v>
       </c>
     </row>
@@ -16344,7 +15928,7 @@
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>26130</v>
       </c>
     </row>
@@ -16352,7 +15936,7 @@
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
         <v>161550</v>
       </c>
     </row>
@@ -20151,7 +19735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10FAB92-64D4-1642-A860-4120FD679806}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -20175,7 +19759,7 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -20276,21 +19860,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B294D875-8478-BA47-87D1-55687F3163D4}">
-  <dimension ref="A3:E16"/>
+  <dimension ref="A3:C12"/>
   <sheetViews>
     <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -20298,225 +19883,64 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3">
       <c r="A5" s="5">
         <v>2011</v>
       </c>
       <c r="B5" s="9">
-        <v>15090</v>
+        <v>8660</v>
       </c>
       <c r="C5" s="9">
         <v>8660</v>
       </c>
-      <c r="D5" s="9">
-        <v>6430</v>
-      </c>
-      <c r="E5" s="9">
-        <v>30180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5">
-        <v>2010</v>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="9">
-        <v>14960</v>
+        <v>8660</v>
       </c>
       <c r="C6" s="9">
-        <v>8610</v>
-      </c>
-      <c r="D6" s="9">
-        <v>6350</v>
-      </c>
-      <c r="E6" s="9">
-        <v>29920</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5">
-        <v>2009</v>
-      </c>
-      <c r="B7" s="9">
-        <v>15110</v>
-      </c>
-      <c r="C7" s="9">
-        <v>8790</v>
-      </c>
-      <c r="D7" s="9">
-        <v>6320</v>
-      </c>
-      <c r="E7" s="9">
-        <v>30220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5">
-        <v>2008</v>
-      </c>
-      <c r="B8" s="9">
-        <v>14100</v>
-      </c>
-      <c r="C8" s="9">
-        <v>7900</v>
-      </c>
-      <c r="D8" s="9">
-        <v>6200</v>
-      </c>
-      <c r="E8" s="9">
-        <v>28200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="5">
-        <v>2007</v>
-      </c>
-      <c r="B9" s="9">
-        <v>13710</v>
-      </c>
-      <c r="C9" s="9">
-        <v>8100</v>
-      </c>
-      <c r="D9" s="9">
-        <v>5610</v>
-      </c>
-      <c r="E9" s="9">
-        <v>27420</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5">
-        <v>2006</v>
-      </c>
-      <c r="B10" s="9">
-        <v>14400</v>
-      </c>
-      <c r="C10" s="9">
-        <v>8540</v>
-      </c>
-      <c r="D10" s="9">
-        <v>5860</v>
-      </c>
-      <c r="E10" s="9">
-        <v>28800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="5">
-        <v>2005</v>
-      </c>
-      <c r="B11" s="9">
-        <v>13960</v>
-      </c>
-      <c r="C11" s="9">
-        <v>7870</v>
-      </c>
-      <c r="D11" s="9">
-        <v>6090</v>
-      </c>
-      <c r="E11" s="9">
-        <v>27920</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="5">
-        <v>2004</v>
-      </c>
-      <c r="B12" s="9">
-        <v>16050</v>
-      </c>
-      <c r="C12" s="9">
-        <v>9940</v>
-      </c>
-      <c r="D12" s="9">
-        <v>6110</v>
-      </c>
-      <c r="E12" s="9">
-        <v>32100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="5">
-        <v>2003</v>
-      </c>
-      <c r="B13" s="9">
-        <v>14160</v>
-      </c>
-      <c r="C13" s="9">
-        <v>8180</v>
-      </c>
-      <c r="D13" s="9">
-        <v>5980</v>
-      </c>
-      <c r="E13" s="9">
-        <v>28320</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="5">
-        <v>2002</v>
-      </c>
-      <c r="B14" s="9">
-        <v>15150</v>
-      </c>
-      <c r="C14" s="9">
-        <v>8590</v>
-      </c>
-      <c r="D14" s="9">
-        <v>6560</v>
-      </c>
-      <c r="E14" s="9">
-        <v>30300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="5">
-        <v>2001</v>
-      </c>
-      <c r="B15" s="9">
-        <v>14860</v>
-      </c>
-      <c r="C15" s="9">
-        <v>8760</v>
-      </c>
-      <c r="D15" s="9">
-        <v>6100</v>
-      </c>
-      <c r="E15" s="9">
-        <v>29720</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="9">
-        <v>161550</v>
-      </c>
-      <c r="C16" s="9">
-        <v>93940</v>
-      </c>
-      <c r="D16" s="9">
-        <v>67610</v>
-      </c>
-      <c r="E16" s="9">
-        <v>323100</v>
+        <v>8660</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f>A5</f>
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
+        <f>B4</f>
+        <v>South</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="str">
+        <f>_xlfn.CONCAT("Sales in ", all_reg_year_and_region_pivot!B11, " by Product - ", all_reg_year_and_region_pivot!B10)</f>
+        <v>Sales in South by Product - 2011</v>
       </c>
     </row>
   </sheetData>
@@ -20527,9 +19951,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC2A83-E1BC-754F-B0D8-8604784CCBBB}">
-  <dimension ref="A3:E11"/>
+  <dimension ref="A3:C11"/>
   <sheetViews>
-    <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -20537,11 +19961,12 @@
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -20549,140 +19974,92 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9">
-        <v>27260</v>
+        <v>1360</v>
       </c>
       <c r="C5" s="9">
-        <v>16140</v>
-      </c>
-      <c r="D5" s="9">
-        <v>11120</v>
-      </c>
-      <c r="E5" s="9">
-        <v>54520</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="9">
-        <v>26770</v>
+        <v>1750</v>
       </c>
       <c r="C6" s="9">
-        <v>15310</v>
-      </c>
-      <c r="D6" s="9">
-        <v>11460</v>
-      </c>
-      <c r="E6" s="9">
-        <v>53540</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="9">
-        <v>26450</v>
+        <v>1020</v>
       </c>
       <c r="C7" s="9">
-        <v>15240</v>
-      </c>
-      <c r="D7" s="9">
-        <v>11210</v>
-      </c>
-      <c r="E7" s="9">
-        <v>52900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="9">
-        <v>26890</v>
+        <v>1070</v>
       </c>
       <c r="C8" s="9">
-        <v>15530</v>
-      </c>
-      <c r="D8" s="9">
-        <v>11360</v>
-      </c>
-      <c r="E8" s="9">
-        <v>53780</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="9">
-        <v>28050</v>
+        <v>1700</v>
       </c>
       <c r="C9" s="9">
-        <v>16530</v>
-      </c>
-      <c r="D9" s="9">
-        <v>11520</v>
-      </c>
-      <c r="E9" s="9">
-        <v>56100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="9">
-        <v>26130</v>
+        <v>1760</v>
       </c>
       <c r="C10" s="9">
-        <v>15190</v>
-      </c>
-      <c r="D10" s="9">
-        <v>10940</v>
-      </c>
-      <c r="E10" s="9">
-        <v>52260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="9">
-        <v>161550</v>
+        <v>8660</v>
       </c>
       <c r="C11" s="9">
-        <v>93940</v>
-      </c>
-      <c r="D11" s="9">
-        <v>67610</v>
-      </c>
-      <c r="E11" s="9">
-        <v>323100</v>
+        <v>8660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a dynamic title and a manual legend to the final dashboard.
</commit_message>
<xml_diff>
--- a/excel_dashboards_challenge.xlsx
+++ b/excel_dashboards_challenge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanferns/Documents/Data_Science/lighthouse_labs_training/DS_auticon_dataviz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E173C-B7B5-894D-81C7-1BF6BCFA60FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C753BF3C-CB41-5341-B6F1-AE2B96D3881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,8 +48,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId11"/>
-    <pivotCache cacheId="5" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -4579,14 +4579,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Sales</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> by Product and Region</a:t>
-            </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
@@ -5534,6 +5526,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
   <c:extLst>
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
@@ -9972,18 +9965,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>16455</xdr:rowOff>
+      <xdr:colOff>137102</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>167989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>505113</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28865</xdr:rowOff>
+      <xdr:colOff>541193</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Region 1">
@@ -10006,7 +9999,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -10016,8 +10009,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4050148"/>
-              <a:ext cx="1327727" cy="1138092"/>
+              <a:off x="137102" y="4014069"/>
+              <a:ext cx="1226705" cy="1138092"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -10047,7 +10040,259 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>21648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>137102</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>137102</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1E887F8-4FC3-48BB-F43F-E2B14C680ADA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4242955"/>
+          <a:ext cx="137102" cy="303067"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>122669</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>49193</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08165922-A241-82AC-E388-B3EF5CE23BC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4531589"/>
+          <a:ext cx="137160" cy="301752"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>43291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>129886</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>7215</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D44F7D42-6D95-62F5-7454-D6979F9210AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4827439"/>
+          <a:ext cx="129886" cy="339151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.12228</cdr:x>
+      <cdr:y>0.00302</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.89893</cdr:x>
+      <cdr:y>0.0625</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="all_reg_year_and_region_pivot!$B$12">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3E35E4-834E-1FE7-8F26-F5BDCBD84CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="923636" y="21648"/>
+          <a:ext cx="5866534" cy="425739"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:fld id="{B5BAE18E-47E1-5B4B-8EB9-705FF7CE4EAB}" type="TxLink">
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Sales in South by Product - 2011</a:t>
+          </a:fld>
+          <a:endParaRPr lang="en-US" sz="2000" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12536,7 +12781,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12710,7 +12955,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0">
@@ -12823,7 +13068,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27187173-58F9-8548-A30F-6078862BE245}" name="AllRegions&amp;YearPivot" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27187173-58F9-8548-A30F-6078862BE245}" name="AllRegions&amp;YearPivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12947,7 +13192,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{587A5213-1027-174C-93A9-DE62478DE20F}" name="Product&amp;RegionPivot" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{587A5213-1027-174C-93A9-DE62478DE20F}" name="Product&amp;RegionPivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0">
@@ -13254,7 +13499,7 @@
 
 <file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Year 1" xr10:uid="{38DD5498-9402-804C-B8E7-A3CA7EC6D120}" cache="Slicer_Year1" caption="Year" rowHeight="230716"/>
+  <slicer name="Year 1" xr10:uid="{38DD5498-9402-804C-B8E7-A3CA7EC6D120}" cache="Slicer_Year1" caption="Pick a year" rowHeight="230716"/>
   <slicer name="Region 1" xr10:uid="{436B51DB-1D6A-CD47-97D3-105DACA7702A}" cache="Slicer_Region1" caption="Region" rowHeight="230716"/>
 </slicers>
 </file>
@@ -15461,8 +15706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE7D515-685B-0547-83BA-13F164C46B95}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Removed legend from the pivot chart on the final dashboard.  Completed final dashboard for now.
</commit_message>
<xml_diff>
--- a/excel_dashboards_challenge.xlsx
+++ b/excel_dashboards_challenge.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanferns/Documents/Data_Science/lighthouse_labs_training/DS_auticon_dataviz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C753BF3C-CB41-5341-B6F1-AE2B96D3881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D083E0-EF6B-0C44-BCDE-EF0CDB22EFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,8 +48,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
-    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -697,7 +697,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-A955-CA46-B653-4F018A158DC5}"/>
+              <c16:uniqueId val="{00000000-D126-1A4E-A357-D8B204BD0DB6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2836,7 +2836,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-9D4A-C340-A2D7-B5997D059235}"/>
+              <c16:uniqueId val="{00000001-B1B1-A945-B0FC-2DD12D7830EF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4068,7 +4068,7 @@
         <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="FF0000"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -4143,7 +4143,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -5454,37 +5454,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5533,7 +5502,6 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -9975,8 +9943,8 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>180400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Region 1">
@@ -9999,7 +9967,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -10285,6 +10253,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>Sales in South by Product - 2011</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1"/>
@@ -12781,7 +12750,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9773013-2BDD-784D-A83F-D8AFF7ED7C0D}" name="Year&amp;RegionPivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="A3:D16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -12955,7 +12924,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86BF2C53-BC0B-754D-8C7A-8158D1D11B67}" name="ProductPivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0">
@@ -13068,7 +13037,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27187173-58F9-8548-A30F-6078862BE245}" name="AllRegions&amp;YearPivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27187173-58F9-8548-A30F-6078862BE245}" name="AllRegions&amp;YearPivot" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -13192,7 +13161,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{587A5213-1027-174C-93A9-DE62478DE20F}" name="Product&amp;RegionPivot" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{587A5213-1027-174C-93A9-DE62478DE20F}" name="Product&amp;RegionPivot" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0">
@@ -20108,7 +20077,7 @@
   <dimension ref="A3:C12"/>
   <sheetViews>
     <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>